<commit_message>
modified sequence & state machine diagrams, ppt file
</commit_message>
<xml_diff>
--- a/문서/191126 설계/간트 차트_수정.xlsx
+++ b/문서/191126 설계/간트 차트_수정.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\최준영\학교\과제, 실습\2학년 2학기 (2019)\소프트웨어 설계(정설영)\191125 설계발표\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyungsook\Desktop\쑥\2019 2학기\소프트웨어 설계\팀프로젝트\SD_2019_2_team7\문서\191126 설계\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DAFC15-9FD8-4D30-A8A4-D7F866E979F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D47DC61-6B6E-45AF-9D5E-A1C1B52D85EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A5335E2C-64F0-4936-B28B-08D34DEC03C8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{A5335E2C-64F0-4936-B28B-08D34DEC03C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="53">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -537,146 +537,69 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color theme="0" tint="-0.499984740745262"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -783,32 +706,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -1058,6 +955,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1076,7 +997,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1101,15 +1022,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1119,278 +1031,272 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="3" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="3" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="3" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="3" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="41" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="42" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="43" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="3" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="3" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="3" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="3" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="50" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="51" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="52" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="47" xfId="4" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1712,73 +1618,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9CE2A9-33F4-4BD6-830E-6BE33B2B69F5}">
   <dimension ref="B2:X37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.125" customWidth="1"/>
-    <col min="2" max="2" width="11.625" customWidth="1"/>
-    <col min="3" max="3" width="20.375" customWidth="1"/>
-    <col min="4" max="4" width="58.25" customWidth="1"/>
-    <col min="5" max="5" width="26.125" customWidth="1"/>
-    <col min="6" max="6" width="19.75" customWidth="1"/>
+    <col min="1" max="1" width="12.09765625" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.3984375" customWidth="1"/>
+    <col min="4" max="4" width="56.69921875" customWidth="1"/>
+    <col min="5" max="5" width="26.09765625" customWidth="1"/>
+    <col min="6" max="6" width="19.69921875" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B3" s="61" t="s">
+    <row r="2" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B3" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="88" t="s">
+      <c r="C3" s="53"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="64"/>
-      <c r="G3" s="92" t="s">
+      <c r="F3" s="55"/>
+      <c r="G3" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="92"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="92" t="s">
+      <c r="H3" s="90"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="92" t="s">
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="91" t="s">
+      <c r="P3" s="90"/>
+      <c r="Q3" s="90"/>
+      <c r="R3" s="90"/>
+      <c r="S3" s="94"/>
+      <c r="T3" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="92"/>
-      <c r="V3" s="93"/>
-      <c r="W3" s="13"/>
+      <c r="U3" s="90"/>
+      <c r="V3" s="91"/>
+      <c r="W3" s="10"/>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B4" s="65"/>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B4" s="56"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="59" t="s">
+      <c r="E4" s="88"/>
+      <c r="F4" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="95" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="5" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -1793,7 +1699,7 @@
       <c r="M4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="O4" s="2" t="s">
@@ -1808,145 +1714,145 @@
       <c r="R4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="S4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="V4" s="66" t="s">
+      <c r="V4" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="W4" s="12"/>
-      <c r="X4" s="11"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="8"/>
     </row>
-    <row r="5" spans="2:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="67" t="s">
+    <row r="5" spans="2:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="103" t="s">
+      <c r="F5" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="21" t="s">
+      <c r="G5" s="96"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="21" t="s">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="96" t="s">
+      <c r="N5" s="97"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="T5" s="18"/>
-      <c r="U5" s="21" t="s">
+      <c r="T5" s="11"/>
+      <c r="U5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="V5" s="68" t="s">
+      <c r="V5" s="59" t="s">
         <v>40</v>
       </c>
       <c r="W5" s="6"/>
       <c r="X5" s="6"/>
     </row>
-    <row r="6" spans="2:24" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="85" t="s">
+    <row r="6" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="25" t="s">
+      <c r="D6" s="15"/>
+      <c r="E6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="103" t="s">
+      <c r="F6" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="9"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="4"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="15"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="6"/>
       <c r="U6" s="6"/>
-      <c r="V6" s="69"/>
+      <c r="V6" s="60"/>
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
     </row>
-    <row r="7" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="86"/>
-      <c r="C7" s="58" t="s">
+    <row r="7" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="85"/>
+      <c r="C7" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="27" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="37"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="9"/>
+      <c r="I7" s="3"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="9"/>
+      <c r="N7" s="4"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="15"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="6"/>
       <c r="U7" s="6"/>
-      <c r="V7" s="70"/>
+      <c r="V7" s="61"/>
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
     </row>
-    <row r="8" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="86"/>
-      <c r="C8" s="58" t="s">
+    <row r="8" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="85"/>
+      <c r="C8" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="27" t="s">
+      <c r="D8" s="15"/>
+      <c r="E8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="98" t="s">
+      <c r="F8" s="77" t="s">
         <v>60</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="9"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="41"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -1956,31 +1862,31 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="15"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="6"/>
       <c r="U8" s="6"/>
-      <c r="V8" s="70"/>
+      <c r="V8" s="61"/>
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
     </row>
-    <row r="9" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="86"/>
-      <c r="C9" s="90" t="s">
+    <row r="9" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="85"/>
+      <c r="C9" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="98" t="s">
+      <c r="F9" s="77" t="s">
         <v>54</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="39"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
@@ -1989,30 +1895,30 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="15"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="6"/>
       <c r="U9" s="6"/>
-      <c r="V9" s="70"/>
+      <c r="V9" s="61"/>
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
     </row>
-    <row r="10" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="86"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="23" t="s">
+    <row r="10" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="85"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="98" t="s">
+      <c r="F10" s="77" t="s">
         <v>55</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="4"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="37"/>
+      <c r="K10" s="29"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="4"/>
@@ -2020,23 +1926,23 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="15"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="6"/>
       <c r="U10" s="6"/>
-      <c r="V10" s="70"/>
+      <c r="V10" s="61"/>
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
     </row>
-    <row r="11" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="86"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="23" t="s">
+    <row r="11" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="85"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="98" t="s">
+      <c r="F11" s="77" t="s">
         <v>65</v>
       </c>
       <c r="G11" s="6"/>
@@ -2044,63 +1950,63 @@
       <c r="I11" s="4"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="52"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="44"/>
       <c r="N11" s="4"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="15"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="6"/>
       <c r="U11" s="6"/>
-      <c r="V11" s="70"/>
+      <c r="V11" s="61"/>
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
     </row>
-    <row r="12" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="85" t="s">
+    <row r="12" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25" t="s">
+      <c r="D12" s="16"/>
+      <c r="E12" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="103" t="s">
+      <c r="F12" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="50"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="69"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="60"/>
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
     </row>
-    <row r="13" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="86"/>
-      <c r="C13" s="58" t="s">
+    <row r="13" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="85"/>
+      <c r="C13" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="27" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="98" t="s">
+      <c r="F13" s="77" t="s">
         <v>57</v>
       </c>
       <c r="G13" s="6"/>
@@ -2110,30 +2016,30 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="39"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="31"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="15"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="6"/>
       <c r="U13" s="6"/>
-      <c r="V13" s="70"/>
+      <c r="V13" s="61"/>
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
     </row>
-    <row r="14" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="86"/>
-      <c r="C14" s="90" t="s">
+    <row r="14" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="85"/>
+      <c r="C14" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="98" t="s">
+      <c r="F14" s="77" t="s">
         <v>55</v>
       </c>
       <c r="G14" s="6"/>
@@ -2145,26 +2051,26 @@
       <c r="M14" s="6"/>
       <c r="N14" s="4"/>
       <c r="O14" s="6"/>
-      <c r="P14" s="37"/>
+      <c r="P14" s="29"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="15"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="6"/>
       <c r="U14" s="6"/>
-      <c r="V14" s="70"/>
+      <c r="V14" s="61"/>
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
     </row>
-    <row r="15" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="86"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="23" t="s">
+    <row r="15" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="85"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="98" t="s">
+      <c r="F15" s="77" t="s">
         <v>56</v>
       </c>
       <c r="G15" s="6"/>
@@ -2176,28 +2082,28 @@
       <c r="M15" s="6"/>
       <c r="N15" s="4"/>
       <c r="O15" s="6"/>
-      <c r="P15" s="37"/>
+      <c r="P15" s="29"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="15"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="6"/>
       <c r="U15" s="6"/>
-      <c r="V15" s="70"/>
+      <c r="V15" s="61"/>
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
     </row>
-    <row r="16" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="86"/>
-      <c r="C16" s="90" t="s">
+    <row r="16" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="85"/>
+      <c r="C16" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="98" t="s">
+      <c r="F16" s="77" t="s">
         <v>58</v>
       </c>
       <c r="G16" s="6"/>
@@ -2210,89 +2116,89 @@
       <c r="N16" s="4"/>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
-      <c r="Q16" s="37"/>
+      <c r="Q16" s="29"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="15"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="6"/>
       <c r="U16" s="6"/>
-      <c r="V16" s="70"/>
+      <c r="V16" s="61"/>
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
     </row>
-    <row r="17" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="87"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="23" t="s">
+    <row r="17" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="86"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="60" t="s">
+      <c r="F17" s="51" t="s">
         <v>59</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="49"/>
+      <c r="I17" s="41"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="49"/>
+      <c r="N17" s="41"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="37"/>
+      <c r="Q17" s="29"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="20"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="1"/>
       <c r="U17" s="1"/>
-      <c r="V17" s="71"/>
+      <c r="V17" s="62"/>
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
     </row>
-    <row r="18" spans="2:24" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="85" t="s">
+    <row r="18" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="48" t="s">
+      <c r="D18" s="16"/>
+      <c r="E18" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="104" t="s">
+      <c r="F18" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
-      <c r="T18" s="33"/>
-      <c r="U18" s="33"/>
-      <c r="V18" s="72"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="25"/>
+      <c r="U18" s="25"/>
+      <c r="V18" s="63"/>
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
     </row>
-    <row r="19" spans="2:24" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="86"/>
-      <c r="C19" s="30" t="s">
+    <row r="19" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="85"/>
+      <c r="C19" s="22" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="57" t="s">
+      <c r="E19" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="F19" s="48" t="s">
         <v>54</v>
       </c>
       <c r="G19" s="6"/>
@@ -2303,27 +2209,27 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="44"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-      <c r="U19" s="45"/>
-      <c r="V19" s="73"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="64"/>
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B20" s="86"/>
-      <c r="C20" s="30" t="s">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B20" s="85"/>
+      <c r="C20" s="22" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="57" t="s">
+      <c r="E20" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="57" t="s">
+      <c r="F20" s="48" t="s">
         <v>55</v>
       </c>
       <c r="G20" s="6"/>
@@ -2334,25 +2240,25 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="4"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="56"/>
-      <c r="U20" s="56"/>
-      <c r="V20" s="74"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="47"/>
+      <c r="U20" s="47"/>
+      <c r="V20" s="65"/>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B21" s="86"/>
-      <c r="C21" s="30" t="s">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B21" s="85"/>
+      <c r="C21" s="22" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="57" t="s">
+      <c r="F21" s="48" t="s">
         <v>56</v>
       </c>
       <c r="G21" s="6"/>
@@ -2364,79 +2270,79 @@
       <c r="M21" s="6"/>
       <c r="N21" s="4"/>
       <c r="O21" s="6"/>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="42"/>
-      <c r="S21" s="42"/>
-      <c r="T21" s="45"/>
-      <c r="U21" s="45"/>
-      <c r="V21" s="73"/>
+      <c r="P21" s="45"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="64"/>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B22" s="87"/>
-      <c r="C22" s="31" t="s">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B22" s="86"/>
+      <c r="C22" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="49"/>
+      <c r="D22" s="41"/>
       <c r="E22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="51" t="s">
         <v>57</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="49"/>
+      <c r="I22" s="41"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="41"/>
-      <c r="S22" s="56"/>
-      <c r="T22" s="102"/>
-      <c r="U22" s="55"/>
-      <c r="V22" s="75"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="33"/>
+      <c r="S22" s="99"/>
+      <c r="T22" s="81"/>
+      <c r="U22" s="46"/>
+      <c r="V22" s="66"/>
     </row>
-    <row r="23" spans="2:24" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="76" t="s">
+    <row r="23" spans="2:24" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="100"/>
-      <c r="E23" s="78" t="s">
+      <c r="C23" s="68"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="99" t="s">
+      <c r="F23" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="G23" s="79"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="80"/>
-      <c r="O23" s="79"/>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="79"/>
-      <c r="S23" s="82"/>
-      <c r="T23" s="101"/>
-      <c r="U23" s="83"/>
-      <c r="V23" s="84"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="70"/>
+      <c r="P23" s="70"/>
+      <c r="Q23" s="70"/>
+      <c r="R23" s="70"/>
+      <c r="S23" s="73"/>
+      <c r="T23" s="80"/>
+      <c r="U23" s="74"/>
+      <c r="V23" s="75"/>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.4">
       <c r="L27" s="7"/>
     </row>
-    <row r="36" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M36" s="22"/>
+    <row r="36" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M36" s="14"/>
     </row>
-    <row r="37" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M37" s="6"/>
     </row>
   </sheetData>

</xml_diff>